<commit_message>
Resolved console errors, added root value bag and formatting options
</commit_message>
<xml_diff>
--- a/documents/Published/JourneyChart/JourneyChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/JourneyChart/JourneyChartByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18518"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sunny\Desktop\Journey Graph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VisualWork\documents\Published\JourneyChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9DC87D1-2946-46F0-8B1D-304B24545FED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{1EF8273B-130D-4D0F-858D-08F8BD12DEF8}"/>
   </bookViews>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>S no</t>
   </si>
@@ -43,10 +44,6 @@
   </si>
   <si>
     <t>Basic Journey chart</t>
-  </si>
-  <si>
-    <t>1. Drag 'Age group' to 'Category Data'
-2. Drag ' 'Joined company' to 'Measure Data'</t>
   </si>
   <si>
     <t>Display basic journey chart</t>
@@ -261,12 +258,51 @@
   <si>
     <t>NA</t>
   </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Power Bi Desktop</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>EDGE</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Change Label Style</t>
+  </si>
+  <si>
+    <t>1. Go to formatting pane
+2. Go to 'Labels' option
+3. Change Label style to Category and value
+4. Change Display units to Thousands and Decimal places to 3</t>
+  </si>
+  <si>
+    <t>1. Values will be displayed along with the category.
+2. Values will display values in K with 3 decimal places</t>
+  </si>
+  <si>
+    <t>1. Drag 'Age group' to 'Category Data'
+2. Drag ' 'Joined company' to 'Measure Data'
+3. Drag any field to 'Root Data' (optional) and go to the format pane -&gt; Root Settings . Select an option either First or Last value.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +333,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -318,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -408,11 +451,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -432,15 +496,35 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -451,7 +535,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -764,9 +849,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F6B169-579D-4921-8F6C-253407ECB244}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -774,112 +861,275 @@
     <col min="3" max="3" width="42.85546875" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="F2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="F7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="E8:E12"/>
+    <mergeCell ref="F8:F12"/>
+    <mergeCell ref="G8:G12"/>
+    <mergeCell ref="H8:H12"/>
+    <mergeCell ref="I8:I12"/>
+    <mergeCell ref="B7:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -888,7 +1138,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,13 +1148,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>24</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -912,10 +1162,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>51</v>
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -923,10 +1173,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>51</v>
+        <v>26</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -934,10 +1184,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>27</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -945,10 +1195,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>51</v>
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -956,10 +1206,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -967,10 +1217,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -978,10 +1228,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>53</v>
+        <v>31</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -989,10 +1239,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1000,10 +1250,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1011,10 +1261,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>51</v>
+        <v>34</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,10 +1272,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>51</v>
+        <v>35</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1033,10 +1283,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>51</v>
+        <v>36</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1044,10 +1294,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>53</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1055,10 +1305,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>51</v>
+        <v>38</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1066,94 +1316,94 @@
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
-        <v>16</v>
-      </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10" t="s">
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="21"/>
+      <c r="B19" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="9"/>
-      <c r="B19" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
-        <v>18</v>
-      </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="22" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="21"/>
+      <c r="B22" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="21"/>
+      <c r="B23" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="13"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="23"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="21"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="23"/>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="21"/>
+      <c r="B25" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="13"/>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="14"/>
+      <c r="C25" s="24"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
         <v>19</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1161,10 +1411,10 @@
         <v>20</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1175,5 +1425,6 @@
     <mergeCell ref="C21:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>